<commit_message>
fill all parameters in BOM
</commit_message>
<xml_diff>
--- a/Project Outputs/BOM/Bill of Materials-BOM.xlsx
+++ b/Project Outputs/BOM/Bill of Materials-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\RF-CONNECTOR\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{572537E7-D58E-409E-8435-549EB6C03519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE863439-AE93-41E7-AA01-7368B329715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{0FE9B602-5015-44E1-95BB-147D287605E8}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{7068DA0C-525E-4845-8AD9-8C0925599E18}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Designator</t>
   </si>
@@ -84,12 +84,18 @@
     <t>RF Connectors / Coaxial Connectors MCX Connector Receptacle, Female Socket 50Ohm Board Edge, Cutout; Surface Mount Solder</t>
   </si>
   <si>
-    <t/>
+    <t>MCX-F</t>
   </si>
   <si>
     <t>-- Linx Technologies Inc.</t>
   </si>
   <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
     <t>B1, B2</t>
   </si>
   <si>
@@ -100,6 +106,9 @@
   </si>
   <si>
     <t>CONN RPSMA PLG STR 50OHM EDGEMNT</t>
+  </si>
+  <si>
+    <t>RP-SMA</t>
   </si>
   <si>
     <t>None</t>
@@ -479,7 +488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AA5AD2-456B-4E87-A8CE-C42DE2B211F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E1A795-5256-4B84-B1D7-CF50D92AB59F}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -556,37 +565,45 @@
       <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update tests to precommit
</commit_message>
<xml_diff>
--- a/Project Outputs/BOM/Bill of Materials-BOM.xlsx
+++ b/Project Outputs/BOM/Bill of Materials-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\RF-CONNECTOR\Project Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D498A86-07A6-4AD4-B872-2DC6F000D232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4598D986-89C2-4EAA-A17B-FD7EFC517BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{15767535-CEEA-4DDA-A70E-1B269AAC5982}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{1AE642A8-7624-4088-A765-950D770D9FD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Designator</t>
   </si>
@@ -491,7 +491,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A5FC75-4EB9-4F41-B2C9-939F7769FE39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{644593C1-4F75-4543-AF1E-BEC658F7EF17}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -574,7 +574,9 @@
       <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
@@ -607,7 +609,9 @@
       <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="K3" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>